<commit_message>
updated with free crm
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/master.xlsx
+++ b/src/test/resources/testdata/master.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasia\eclipse-workspace\Automation\src\test\resources\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C9AE9F-73DC-467A-B732-9264A7CB6E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="TestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>TestCases</t>
   </si>
@@ -37,29 +43,32 @@
     <t>chrome</t>
   </si>
   <si>
-    <t>LoginTest</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
-    <t>ValidateCRMTest</t>
-  </si>
-  <si>
     <t>Admin@123</t>
   </si>
   <si>
-    <t>andrew74444@gmail.com</t>
-  </si>
-  <si>
-    <t>email</t>
+    <t>searchGoogle</t>
+  </si>
+  <si>
+    <t>searchGoogle2</t>
+  </si>
+  <si>
+    <t>SearchKeyword</t>
+  </si>
+  <si>
+    <t>Selenium Automation demo 1</t>
+  </si>
+  <si>
+    <t>Selenium Automation demo 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,23 +371,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,17 +398,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -408,48 +420,81 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>